<commit_message>
Add automation script, add tables to report
</commit_message>
<xml_diff>
--- a/p4-bad.xlsx
+++ b/p4-bad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\PEA\PEA-projekt4-ErykMika-264451\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3547BFE9-08E1-4BE2-AEBD-DA8F53A7B134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F086D4-68F8-4713-BD4A-52C0931FB127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="47_0.01" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="5">
   <si>
     <t>scramble</t>
   </si>
   <si>
     <t>inverse</t>
+  </si>
+  <si>
+    <t>Czas [ms]</t>
+  </si>
+  <si>
+    <t>Koszt ścieżki</t>
+  </si>
+  <si>
+    <t>Błąd [%]</t>
   </si>
 </sst>
 </file>
@@ -101,7 +110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -112,6 +121,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -393,550 +406,894 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1000</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10000</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>100000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
         <v>81561.600000000006</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>2287</v>
       </c>
-      <c r="D3" s="3">
+      <c r="C4" s="7">
+        <f t="shared" ref="C4:C13" si="0">(B4-$M$4)/$M$4</f>
+        <v>0.2877252252252252</v>
+      </c>
+      <c r="E4" s="13">
         <v>4928.21</v>
       </c>
-      <c r="E3">
+      <c r="F4">
         <v>2218</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:G13" si="1">(F4-$M$4)/$M$4</f>
+        <v>0.24887387387387389</v>
+      </c>
+      <c r="I4" s="13">
         <v>12791.8</v>
       </c>
-      <c r="H3" s="5">
+      <c r="J4" s="5">
         <v>2202</v>
       </c>
-      <c r="J3">
+      <c r="K4" s="11">
+        <f t="shared" ref="K4:K13" si="2">(J4-$M$4)/$M$4</f>
+        <v>0.23986486486486486</v>
+      </c>
+      <c r="M4">
         <v>1776</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
         <v>4432.01</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>2234</v>
       </c>
-      <c r="D4" s="3">
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.25788288288288286</v>
+      </c>
+      <c r="E5" s="13">
         <v>1542.91</v>
       </c>
-      <c r="E4">
+      <c r="F5">
         <v>2241</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="7">
+        <f t="shared" si="1"/>
+        <v>0.26182432432432434</v>
+      </c>
+      <c r="I5" s="13">
         <v>20325.599999999999</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J5" s="5">
         <v>2176</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="K5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.22522522522522523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
         <v>68334.3</v>
-      </c>
-      <c r="B5">
-        <v>2287</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1202.57</v>
-      </c>
-      <c r="E5">
-        <v>2217</v>
-      </c>
-      <c r="G5" s="3">
-        <v>97396.2</v>
-      </c>
-      <c r="H5" s="5">
-        <v>2164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>28498.1</v>
       </c>
       <c r="B6">
         <v>2287</v>
       </c>
-      <c r="D6" s="3">
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2877252252252252</v>
+      </c>
+      <c r="E6" s="13">
+        <v>1202.57</v>
+      </c>
+      <c r="F6">
+        <v>2217</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="1"/>
+        <v>0.2483108108108108</v>
+      </c>
+      <c r="I6" s="13">
+        <v>97396.2</v>
+      </c>
+      <c r="J6" s="5">
+        <v>2164</v>
+      </c>
+      <c r="K6" s="11">
+        <f t="shared" si="2"/>
+        <v>0.21846846846846846</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>28498.1</v>
+      </c>
+      <c r="B7">
+        <v>2287</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2877252252252252</v>
+      </c>
+      <c r="E7" s="13">
         <v>1220.55</v>
       </c>
-      <c r="E6">
+      <c r="F7">
         <v>2289</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G7" s="7">
+        <f t="shared" si="1"/>
+        <v>0.28885135135135137</v>
+      </c>
+      <c r="I7" s="13">
         <v>11006</v>
       </c>
-      <c r="H6" s="5">
+      <c r="J7" s="5">
         <v>2217</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="K7" s="11">
+        <f t="shared" si="2"/>
+        <v>0.2483108108108108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
         <v>12822.6</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>2241</v>
       </c>
-      <c r="D7" s="3">
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.26182432432432434</v>
+      </c>
+      <c r="E8" s="13">
         <v>1088.52</v>
       </c>
-      <c r="E7">
+      <c r="F8">
         <v>2234</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G8" s="7">
+        <f t="shared" si="1"/>
+        <v>0.25788288288288286</v>
+      </c>
+      <c r="I8" s="13">
         <v>15547.9</v>
       </c>
-      <c r="H7" s="5">
+      <c r="J8" s="5">
         <v>2218</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="K8" s="11">
+        <f t="shared" si="2"/>
+        <v>0.24887387387387389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
         <v>7449.3</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>2287</v>
       </c>
-      <c r="D8" s="3">
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2877252252252252</v>
+      </c>
+      <c r="E9" s="13">
         <v>895.69200000000001</v>
       </c>
-      <c r="E8">
+      <c r="F9">
         <v>2241</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.26182432432432434</v>
+      </c>
+      <c r="I9" s="13">
         <v>33415</v>
       </c>
-      <c r="H8" s="5">
+      <c r="J9" s="5">
         <v>2173</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="K9" s="11">
+        <f t="shared" si="2"/>
+        <v>0.22353603603603603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
         <v>15620.5</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>2241</v>
       </c>
-      <c r="D9" s="3">
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.26182432432432434</v>
+      </c>
+      <c r="E10" s="13">
         <v>12646.8</v>
       </c>
-      <c r="E9">
+      <c r="F10">
         <v>2181</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.22804054054054054</v>
+      </c>
+      <c r="I10" s="13">
         <v>11212.7</v>
       </c>
-      <c r="H9" s="5">
+      <c r="J10" s="5">
         <v>2183</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="K10" s="11">
+        <f t="shared" si="2"/>
+        <v>0.22916666666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
         <v>10426.1</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>2234</v>
       </c>
-      <c r="D10" s="3">
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.25788288288288286</v>
+      </c>
+      <c r="E11" s="13">
         <v>58668.2</v>
       </c>
-      <c r="E10">
+      <c r="F11">
         <v>2265</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.27533783783783783</v>
+      </c>
+      <c r="I11" s="13">
         <v>10115.700000000001</v>
       </c>
-      <c r="H10" s="5">
+      <c r="J11" s="5">
         <v>2183</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="K11" s="11">
+        <f t="shared" si="2"/>
+        <v>0.22916666666666666</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
         <v>48213.2</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>2287</v>
       </c>
-      <c r="D11" s="3">
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2877252252252252</v>
+      </c>
+      <c r="E12" s="13">
         <v>1246.19</v>
       </c>
-      <c r="E11">
+      <c r="F12">
         <v>2234</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.25788288288288286</v>
+      </c>
+      <c r="I12" s="13">
         <v>8813.49</v>
       </c>
-      <c r="H11" s="5">
+      <c r="J12" s="5">
         <v>2234</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="K12" s="11">
+        <f t="shared" si="2"/>
+        <v>0.25788288288288286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
         <v>9168.01</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>2241</v>
       </c>
-      <c r="D12" s="3">
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.26182432432432434</v>
+      </c>
+      <c r="E13" s="13">
         <v>46916</v>
       </c>
-      <c r="E12">
+      <c r="F13">
         <v>2202</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.23986486486486486</v>
+      </c>
+      <c r="I13" s="13">
         <v>37586.1</v>
       </c>
-      <c r="H12" s="5">
+      <c r="J13" s="5">
         <v>2145</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <f>AVERAGE(A3:A12)</f>
+      <c r="K13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.20777027027027026</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <f>AVERAGE(A4:A13)</f>
         <v>28652.572000000004</v>
       </c>
-      <c r="B13" s="2">
-        <f>AVERAGE(B3:B12)</f>
+      <c r="B14" s="2">
+        <f>AVERAGE(B4:B13)</f>
         <v>2262.6</v>
       </c>
-      <c r="D13" s="4">
-        <f>AVERAGE(D3:D12)</f>
+      <c r="C14" s="10">
+        <f>AVERAGE(C4:C13)</f>
+        <v>0.27398648648648649</v>
+      </c>
+      <c r="E14" s="4">
+        <f>AVERAGE(E4:E13)</f>
         <v>13035.564199999999</v>
       </c>
-      <c r="E13" s="2">
-        <f>AVERAGE(E3:E12)</f>
+      <c r="F14" s="2">
+        <f>AVERAGE(F4:F13)</f>
         <v>2232.1999999999998</v>
       </c>
-      <c r="G13" s="4">
-        <f>AVERAGE(G3:G12)</f>
+      <c r="G14" s="10">
+        <f>AVERAGE(G4:G13)</f>
+        <v>0.25686936936936933</v>
+      </c>
+      <c r="I14" s="4">
+        <f>AVERAGE(I4:I13)</f>
         <v>25821.048999999999</v>
       </c>
-      <c r="H13" s="2">
-        <f>AVERAGE(H3:H12)</f>
+      <c r="J14" s="2">
+        <f>AVERAGE(J4:J13)</f>
         <v>2189.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="6">
-        <f>(B13-$J$3)/$J$3</f>
+      <c r="K14" s="12">
+        <f>AVERAGE(K4:K13)</f>
+        <v>0.2328265765765766</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="11">
+        <f>(B14-$M$4)/$M$4</f>
         <v>0.27398648648648644</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6">
-        <f>(E13-$J$3)/$J$3</f>
+      <c r="C15" s="7"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11">
+        <f>(F14-$M$4)/$M$4</f>
         <v>0.25686936936936927</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6">
-        <f>(H13-$J$3)/$J$3</f>
+      <c r="G15" s="7"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11">
+        <f>(J14-$M$4)/$M$4</f>
         <v>0.23282657657657657</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="C17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>102113</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>2130</v>
       </c>
-      <c r="D17" s="3">
+      <c r="C19" s="7">
+        <f t="shared" ref="C19:C28" si="3">(B19-$M$4)/$M$4</f>
+        <v>0.19932432432432431</v>
+      </c>
+      <c r="E19" s="3">
         <v>95816.6</v>
       </c>
-      <c r="E17">
+      <c r="F19">
         <v>2183</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G19" s="7">
+        <f t="shared" ref="G19:G28" si="4">(F19-$M$4)/$M$4</f>
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="I19" s="3">
         <v>13367.5</v>
       </c>
-      <c r="H17">
+      <c r="J19">
         <v>2135</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="K19" s="11">
+        <f t="shared" ref="K19:K28" si="5">(J19-$M$4)/$M$4</f>
+        <v>0.20213963963963963</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>2690.94</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>2234</v>
       </c>
-      <c r="D18" s="3">
+      <c r="C20" s="7">
+        <f t="shared" si="3"/>
+        <v>0.25788288288288286</v>
+      </c>
+      <c r="E20" s="3">
         <v>113808</v>
       </c>
-      <c r="E18">
+      <c r="F20">
         <v>2183</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="I20" s="3">
         <v>38633.300000000003</v>
       </c>
-      <c r="H18">
+      <c r="J20">
         <v>2234</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="K20" s="11">
+        <f t="shared" si="5"/>
+        <v>0.25788288288288286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>5886.06</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>2210</v>
       </c>
-      <c r="D19" s="3">
+      <c r="C21" s="7">
+        <f t="shared" si="3"/>
+        <v>0.24436936936936937</v>
+      </c>
+      <c r="E21" s="3">
         <v>106887</v>
       </c>
-      <c r="E19">
+      <c r="F21">
         <v>2170</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G21" s="7">
+        <f t="shared" si="4"/>
+        <v>0.22184684684684686</v>
+      </c>
+      <c r="I21" s="3">
         <v>116273</v>
       </c>
-      <c r="H19">
+      <c r="J21">
         <v>2175</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="K21" s="11">
+        <f t="shared" si="5"/>
+        <v>0.22466216216216217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>29365.200000000001</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>2199</v>
       </c>
-      <c r="D20" s="3">
+      <c r="C22" s="7">
+        <f t="shared" si="3"/>
+        <v>0.23817567567567569</v>
+      </c>
+      <c r="E22" s="3">
         <v>82506</v>
       </c>
-      <c r="E20">
+      <c r="F22">
         <v>2165</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G22" s="7">
+        <f t="shared" si="4"/>
+        <v>0.21903153153153154</v>
+      </c>
+      <c r="I22" s="3">
         <v>116311</v>
       </c>
-      <c r="H20">
+      <c r="J22">
         <v>2122</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="K22" s="11">
+        <f t="shared" si="5"/>
+        <v>0.19481981981981983</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>71253.3</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>2181</v>
       </c>
-      <c r="D21" s="3">
+      <c r="C23" s="7">
+        <f t="shared" si="3"/>
+        <v>0.22804054054054054</v>
+      </c>
+      <c r="E23" s="3">
         <v>81700.2</v>
       </c>
-      <c r="E21">
+      <c r="F23">
         <v>2146</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G23" s="7">
+        <f t="shared" si="4"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I23" s="3">
         <v>15493.3</v>
       </c>
-      <c r="H21">
+      <c r="J23">
         <v>2215</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="K23" s="11">
+        <f t="shared" si="5"/>
+        <v>0.24718468468468469</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>48952.1</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>2195</v>
       </c>
-      <c r="D22" s="3">
+      <c r="C24" s="7">
+        <f t="shared" si="3"/>
+        <v>0.23592342342342343</v>
+      </c>
+      <c r="E24" s="3">
         <v>6605.61</v>
       </c>
-      <c r="E22">
+      <c r="F24">
         <v>2218</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G24" s="7">
+        <f t="shared" si="4"/>
+        <v>0.24887387387387389</v>
+      </c>
+      <c r="I24" s="3">
         <v>97062.399999999994</v>
       </c>
-      <c r="H22">
+      <c r="J24">
         <v>2217</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="K24" s="11">
+        <f t="shared" si="5"/>
+        <v>0.2483108108108108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>98612.4</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>2199</v>
       </c>
-      <c r="D23" s="3">
+      <c r="C25" s="7">
+        <f t="shared" si="3"/>
+        <v>0.23817567567567569</v>
+      </c>
+      <c r="E25" s="3">
         <v>45547</v>
       </c>
-      <c r="E23">
+      <c r="F25">
         <v>2170</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G25" s="7">
+        <f t="shared" si="4"/>
+        <v>0.22184684684684686</v>
+      </c>
+      <c r="I25" s="3">
         <v>8636.4500000000007</v>
       </c>
-      <c r="H23">
+      <c r="J25">
         <v>2234</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="K25" s="11">
+        <f t="shared" si="5"/>
+        <v>0.25788288288288286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>95018.3</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>2210</v>
       </c>
-      <c r="D24" s="3">
+      <c r="C26" s="7">
+        <f t="shared" si="3"/>
+        <v>0.24436936936936937</v>
+      </c>
+      <c r="E26" s="3">
         <v>80067</v>
       </c>
-      <c r="E24">
+      <c r="F26">
         <v>2141</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G26" s="7">
+        <f t="shared" si="4"/>
+        <v>0.20551801801801803</v>
+      </c>
+      <c r="I26" s="3">
         <v>18288.900000000001</v>
       </c>
-      <c r="H24">
+      <c r="J26">
         <v>2194</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="K26" s="11">
+        <f t="shared" si="5"/>
+        <v>0.23536036036036037</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>52846.1</v>
       </c>
-      <c r="B25">
+      <c r="B27">
         <v>2176</v>
       </c>
-      <c r="D25" s="3">
+      <c r="C27" s="7">
+        <f t="shared" si="3"/>
+        <v>0.22522522522522523</v>
+      </c>
+      <c r="E27" s="3">
         <v>91701.9</v>
       </c>
-      <c r="E25">
+      <c r="F27">
         <v>2146</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G27" s="7">
+        <f t="shared" si="4"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I27" s="3">
         <v>10281.6</v>
       </c>
-      <c r="H25">
+      <c r="J27">
         <v>2183</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="K27" s="11">
+        <f t="shared" si="5"/>
+        <v>0.22916666666666666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>18607.900000000001</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>2273</v>
       </c>
-      <c r="D26" s="3">
+      <c r="C28" s="7">
+        <f t="shared" si="3"/>
+        <v>0.27984234234234234</v>
+      </c>
+      <c r="E28" s="3">
         <v>1136.2</v>
       </c>
-      <c r="E26">
+      <c r="F28">
         <v>2243</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G28" s="7">
+        <f t="shared" si="4"/>
+        <v>0.26295045045045046</v>
+      </c>
+      <c r="I28" s="3">
         <v>10229</v>
       </c>
-      <c r="H26">
+      <c r="J28">
         <v>2217</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
-        <f>AVERAGE(A17:A26)</f>
+      <c r="K28" s="11">
+        <f t="shared" si="5"/>
+        <v>0.2483108108108108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <f>AVERAGE(A19:A28)</f>
         <v>52534.529999999992</v>
       </c>
-      <c r="B27" s="2">
-        <f t="shared" ref="B27" si="0">AVERAGE(B17:B26)</f>
+      <c r="B29" s="2">
+        <f t="shared" ref="B29" si="6">AVERAGE(B19:B28)</f>
         <v>2200.6999999999998</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4">
-        <f>AVERAGE(D17:D26)</f>
+      <c r="C29" s="12">
+        <f>AVERAGE(C19:C28)</f>
+        <v>0.23913288288288287</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4">
+        <f>AVERAGE(E19:E28)</f>
         <v>70577.550999999992</v>
       </c>
-      <c r="E27" s="2">
-        <f>AVERAGE(E17:E26)</f>
+      <c r="F29" s="2">
+        <f>AVERAGE(F19:F28)</f>
         <v>2176.5</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4">
-        <f>AVERAGE(G17:G26)</f>
+      <c r="G29" s="12">
+        <f>AVERAGE(G19:G28)</f>
+        <v>0.22550675675675674</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4">
+        <f>AVERAGE(I19:I28)</f>
         <v>44457.645000000004</v>
       </c>
-      <c r="H27" s="2">
-        <f>AVERAGE(H17:H26)</f>
+      <c r="J29" s="2">
+        <f>AVERAGE(J19:J28)</f>
         <v>2192.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6">
-        <f>(B27-$J$3)/$J$3</f>
+      <c r="K29" s="12">
+        <f>AVERAGE(K19:K28)</f>
+        <v>0.23457207207207209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="11">
+        <f>(B29-$M$4)/$M$4</f>
         <v>0.23913288288288279</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6">
-        <f>(E27-$J$3)/$J$3</f>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11">
+        <f>(F29-$M$4)/$M$4</f>
         <v>0.22550675675675674</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6">
-        <f>(H27-$J$3)/$J$3</f>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11">
+        <f>(J29-$M$4)/$M$4</f>
         <v>0.23457207207207201</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="7">
-        <f>(B14+B28)/2</f>
+      <c r="K30" s="11"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="7">
+        <f>(B15+B30)/2</f>
         <v>0.2565596846846846</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7">
-        <f>(E14+E28)/2</f>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7">
+        <f>(F15+F30)/2</f>
         <v>0.24118806306306301</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="9">
-        <f>(H14+H28)/2</f>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="9">
+        <f>(J15+J30)/2</f>
         <v>0.23369932432432428</v>
       </c>
+      <c r="K32" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1313,7 +1670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7656AF5D-CCA4-4A30-AC89-9F5B9C27E981}">
   <dimension ref="A2:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -1611,7 +1968,7 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6">
-        <f t="shared" ref="C18:H18" si="2">(E17-$J$4)/$J$4</f>
+        <f t="shared" ref="E18:H18" si="2">(E17-$J$4)/$J$4</f>
         <v>0.26807302231237329</v>
       </c>
       <c r="F18" s="6"/>

</xml_diff>